<commit_message>
programing procedure, elchem board
</commit_message>
<xml_diff>
--- a/2-Electrical/0 - Development Drawings/3-SensorTGS2xxx_board/2-BOM/BOMs_Sensor_board_v1.1_allVariants.xlsx
+++ b/2-Electrical/0 - Development Drawings/3-SensorTGS2xxx_board/2-BOM/BOMs_Sensor_board_v1.1_allVariants.xlsx
@@ -11,7 +11,7 @@
     <sheet name="varA" sheetId="2" r:id="rId2"/>
     <sheet name="varB" sheetId="3" r:id="rId3"/>
     <sheet name="varC" sheetId="4" r:id="rId4"/>
-    <sheet name="Hárok1" sheetId="5" r:id="rId5"/>
+    <sheet name="Changelist" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Assembly_partlist_all_v1" localSheetId="0">coordinates_all_variants!$A$1:$F$29</definedName>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="122">
   <si>
     <t>Part</t>
   </si>
@@ -455,9 +455,6 @@
     <t>V1.1</t>
   </si>
   <si>
-    <t>C13 changed from 100n to 1n</t>
-  </si>
-  <si>
     <t>C1(DNP), C2, C3</t>
   </si>
   <si>
@@ -471,6 +468,15 @@
   </si>
   <si>
     <t>C9(DNP), C10(DNP), C13(DNP)</t>
+  </si>
+  <si>
+    <t>C13 changed from 100n to 1n, added assembly side column</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>TOP</t>
   </si>
 </sst>
 </file>
@@ -873,9 +879,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -885,11 +893,12 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -910,10 +919,14 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -933,10 +946,13 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -956,10 +972,13 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -979,10 +998,13 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1002,10 +1024,13 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1025,10 +1050,13 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1047,11 +1075,14 @@
       <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1068,10 +1099,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1088,10 +1122,13 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1111,10 +1148,13 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1134,10 +1174,13 @@
         <v>9</v>
       </c>
       <c r="H11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1157,10 +1200,13 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1180,10 +1226,13 @@
         <v>14</v>
       </c>
       <c r="H13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1203,10 +1252,13 @@
         <v>14</v>
       </c>
       <c r="H14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1226,10 +1278,13 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1249,10 +1304,13 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1272,10 +1330,13 @@
         <v>7</v>
       </c>
       <c r="H17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1295,10 +1356,13 @@
         <v>37</v>
       </c>
       <c r="H18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1318,10 +1382,13 @@
         <v>14</v>
       </c>
       <c r="H19" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1341,10 +1408,13 @@
         <v>14</v>
       </c>
       <c r="H20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1364,10 +1434,13 @@
         <v>14</v>
       </c>
       <c r="H21" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1387,10 +1460,13 @@
         <v>14</v>
       </c>
       <c r="H22" t="s">
+        <v>121</v>
+      </c>
+      <c r="I22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1410,10 +1486,13 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1433,10 +1512,13 @@
         <v>37</v>
       </c>
       <c r="H24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1456,10 +1538,13 @@
         <v>14</v>
       </c>
       <c r="H25" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1479,10 +1564,13 @@
         <v>37</v>
       </c>
       <c r="H26" t="s">
+        <v>121</v>
+      </c>
+      <c r="I26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1502,10 +1590,13 @@
         <v>37</v>
       </c>
       <c r="H27" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1525,10 +1616,13 @@
         <v>9</v>
       </c>
       <c r="H28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1548,6 +1642,9 @@
         <v>53</v>
       </c>
       <c r="H29" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1559,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="I4" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,17 +1672,17 @@
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1610,8 +1707,11 @@
       <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1636,8 +1736,11 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1662,8 +1765,11 @@
       <c r="H6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1685,8 +1791,11 @@
       <c r="H7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1708,8 +1817,11 @@
       <c r="H8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1734,8 +1846,11 @@
       <c r="H9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1760,8 +1875,11 @@
       <c r="H10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1786,8 +1904,11 @@
       <c r="H11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1812,8 +1933,11 @@
       <c r="H12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1838,8 +1962,11 @@
       <c r="H13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1864,8 +1991,11 @@
       <c r="H14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1890,8 +2020,11 @@
       <c r="H15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1915,6 +2048,9 @@
       </c>
       <c r="H16" t="s">
         <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -1987,7 +2123,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,7 +2208,7 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2152,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,17 +2308,17 @@
     <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2210,8 +2346,11 @@
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2236,8 +2375,11 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2262,8 +2404,11 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2288,8 +2433,11 @@
       <c r="I6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2314,8 +2462,11 @@
       <c r="I7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2340,8 +2491,11 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2363,8 +2517,11 @@
       <c r="I9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2386,8 +2543,11 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2412,8 +2572,11 @@
       <c r="I11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2438,8 +2601,11 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2464,8 +2630,11 @@
       <c r="I13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2490,8 +2659,11 @@
       <c r="I14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2516,8 +2688,11 @@
       <c r="I15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2541,6 +2716,9 @@
       </c>
       <c r="I16" t="s">
         <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2568,6 +2746,9 @@
       <c r="I17" t="s">
         <v>7</v>
       </c>
+      <c r="J17" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2594,7 +2775,9 @@
       <c r="I18" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" t="s">
+        <v>121</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
@@ -2623,6 +2806,9 @@
       <c r="I19" t="s">
         <v>14</v>
       </c>
+      <c r="J19" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2649,6 +2835,9 @@
       <c r="I20" t="s">
         <v>14</v>
       </c>
+      <c r="J20" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2675,6 +2864,9 @@
       <c r="I21" t="s">
         <v>37</v>
       </c>
+      <c r="J21" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2701,6 +2893,9 @@
       <c r="I22" t="s">
         <v>37</v>
       </c>
+      <c r="J22" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2727,6 +2922,9 @@
       <c r="I23" t="s">
         <v>37</v>
       </c>
+      <c r="J23" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2753,6 +2951,9 @@
       <c r="I24" t="s">
         <v>9</v>
       </c>
+      <c r="J24" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
@@ -2824,7 +3025,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2909,7 +3110,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,10 +3205,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="I25" sqref="H25:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,19 +3219,20 @@
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3058,8 +3260,11 @@
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3084,8 +3289,11 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3110,8 +3318,11 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3136,8 +3347,11 @@
       <c r="I6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3159,8 +3373,11 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3185,8 +3402,11 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -3211,8 +3431,11 @@
       <c r="I9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3237,8 +3460,11 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3263,8 +3489,11 @@
       <c r="I11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3289,8 +3518,11 @@
       <c r="I12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -3315,8 +3547,11 @@
       <c r="I13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -3341,8 +3576,11 @@
       <c r="I14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -3367,8 +3605,11 @@
       <c r="I15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -3393,8 +3634,11 @@
       <c r="I16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -3419,8 +3663,11 @@
       <c r="I17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3445,13 +3692,16 @@
       <c r="I18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="J18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -3471,7 +3721,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3485,7 +3735,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3502,7 +3752,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -3516,10 +3766,10 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -3536,7 +3786,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3553,7 +3803,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3570,7 +3820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -3587,7 +3837,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3601,10 +3851,10 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3621,7 +3871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3638,7 +3888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3739,7 +3989,7 @@
         <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>